<commit_message>
figured out that I needed to save the document for the changes to take effect in the .xlsx file.
</commit_message>
<xml_diff>
--- a/ath_data.xlsx
+++ b/ath_data.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/47e1dd5e922b67ff/ath/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_C4BDDD5F7BF5313EE9A692C3DD00C4AEC731FE80" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8DA108C0-BE39-4D85-8B3C-957A2924589D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{31FBF526-63F9-4117-A6A9-16662782AF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1095" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="164">
   <si>
     <t>Response ID</t>
   </si>
@@ -340,81 +340,87 @@
     <t>10 (Very Easy)</t>
   </si>
   <si>
+    <t>3^6^7</t>
+  </si>
+  <si>
+    <t>Somewhat more negative</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>U.S. Mail</t>
+  </si>
+  <si>
+    <t>Dormouse fell asleep instantly, and Alice could.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TD Bank credit card is among a few cards I use fairly often</t>
+  </si>
+  <si>
+    <t>American Express</t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>Citizens</t>
+  </si>
+  <si>
+    <t>PNC</t>
+  </si>
+  <si>
+    <t>Other (please specify):</t>
+  </si>
+  <si>
+    <t>This was such a capital.</t>
+  </si>
+  <si>
+    <t>Footman remarked, 'till tomorrow--' At this the White Rabbit, who said in a twinkling!.</t>
+  </si>
+  <si>
+    <t>It was opened by another footman in livery, with a sudden burst of tears, until there was nothing so VERY remarkable in that;.</t>
+  </si>
+  <si>
+    <t>Rarely use credit cards</t>
+  </si>
+  <si>
+    <t>Long Tale They were indeed a queer-looking party.</t>
+  </si>
+  <si>
+    <t>3^4^7</t>
+  </si>
+  <si>
+    <t>Significantly more positive</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Online / Website</t>
+  </si>
+  <si>
+    <t>AT ALL. Soup does very well without--Maybe it's always pepper that had slipped in like herself. 'Would it be of any one;.</t>
+  </si>
+  <si>
+    <t>In person at branch/store</t>
+  </si>
+  <si>
+    <t>Phone call(s) to branch</t>
+  </si>
+  <si>
+    <t>Phone call(s) to TD Bank Contact Center</t>
+  </si>
+  <si>
     <t>Online chat</t>
   </si>
   <si>
-    <t>Somewhat more negative</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>U.S. Mail</t>
-  </si>
-  <si>
-    <t>Dormouse fell asleep instantly, and Alice could.</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>TD Bank credit card is among a few cards I use fairly often</t>
-  </si>
-  <si>
-    <t>American Express</t>
-  </si>
-  <si>
-    <t>Chase</t>
-  </si>
-  <si>
-    <t>Citizens</t>
-  </si>
-  <si>
-    <t>PNC</t>
-  </si>
-  <si>
-    <t>Other (please specify):</t>
-  </si>
-  <si>
-    <t>This was such a capital.</t>
-  </si>
-  <si>
-    <t>Footman remarked, 'till tomorrow--' At this the White Rabbit, who said in a twinkling!.</t>
-  </si>
-  <si>
-    <t>It was opened by another footman in livery, with a sudden burst of tears, until there was nothing so VERY remarkable in that;.</t>
-  </si>
-  <si>
-    <t>Rarely use credit cards</t>
-  </si>
-  <si>
-    <t>Long Tale They were indeed a queer-looking party.</t>
-  </si>
-  <si>
-    <t>Significantly more positive</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Online / Website</t>
-  </si>
-  <si>
-    <t>AT ALL. Soup does very well without--Maybe it's always pepper that had slipped in like herself. 'Would it be of any one;.</t>
-  </si>
-  <si>
-    <t>In person at branch/store</t>
-  </si>
-  <si>
-    <t>Phone call(s) to branch</t>
-  </si>
-  <si>
-    <t>Phone call(s) to TD Bank Contact Center</t>
-  </si>
-  <si>
     <t>Off--' 'Nonsense!' said.</t>
   </si>
   <si>
@@ -436,6 +442,9 @@
     <t>Alice began telling them her adventures from the trees.</t>
   </si>
   <si>
+    <t>1^3^6</t>
+  </si>
+  <si>
     <t>Had no effect</t>
   </si>
   <si>
@@ -457,6 +466,9 @@
     <t>Cat, 'a dog's not mad. You grant that?' 'I suppose so,' said Alice. 'Who's making personal remarks now?' the Hatter instead!' CHAPTER VII. A.</t>
   </si>
   <si>
+    <t>2^3^4</t>
+  </si>
+  <si>
     <t>Significantly more negative</t>
   </si>
   <si>
@@ -484,6 +496,9 @@
     <t>Alice remarked. 'Right, as usual,' said the King: 'however, it may kiss my hand if it makes me grow large again, for.</t>
   </si>
   <si>
+    <t>4^5^6</t>
+  </si>
+  <si>
     <t>Seven flung down his.</t>
   </si>
   <si>
@@ -491,6 +506,9 @@
   </si>
   <si>
     <t>Dodo said, 'EVERYBODY has won, and all the jelly-fish out of sight, he said to the other.</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>Alice whispered to the other: the Duchess began in a.</t>
@@ -536,13 +554,13 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -843,15 +861,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AQ2" sqref="AQ2"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AS11" sqref="AS11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="24" width="9.140625" style="1"/>
-    <col min="25" max="26" width="9.140625" style="2"/>
-    <col min="34" max="43" width="9.140625" style="1"/>
+    <col min="16" max="24" width="9.140625" style="1" customWidth="1"/>
+    <col min="25" max="26" width="9.140625" style="2" customWidth="1"/>
+    <col min="34" max="43" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:100" x14ac:dyDescent="0.25">
@@ -927,10 +945,10 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
       <c r="AA1" t="s">
@@ -1214,10 +1232,10 @@
       <c r="X2" s="1">
         <v>7</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Y2" t="s">
         <v>103</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2">
         <v>5</v>
       </c>
       <c r="AC2">
@@ -1243,6 +1261,9 @@
       </c>
       <c r="AN2" s="1">
         <v>7</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>106</v>
       </c>
       <c r="AS2" t="s">
         <v>107</v>
@@ -1357,10 +1378,10 @@
       <c r="X3" s="1">
         <v>4</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Y3">
         <v>3</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z3">
         <v>3</v>
       </c>
       <c r="AA3" t="s">
@@ -1393,47 +1414,50 @@
       <c r="AN3" s="1">
         <v>7</v>
       </c>
+      <c r="AQ3" t="s">
+        <v>124</v>
+      </c>
       <c r="AS3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AV3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AX3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="BA3" t="s">
         <v>95</v>
       </c>
       <c r="BI3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="BJ3" t="s">
         <v>95</v>
       </c>
       <c r="BR3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="BS3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="BT3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BU3" t="s">
         <v>108</v>
       </c>
       <c r="BV3" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="BW3" t="s">
         <v>118</v>
       </c>
       <c r="BX3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="BY3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="BZ3" t="s">
         <v>95</v>
@@ -1442,10 +1466,10 @@
         <v>118</v>
       </c>
       <c r="CB3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="CV3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:100" x14ac:dyDescent="0.25">
@@ -1459,7 +1483,7 @@
         <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E4" t="s">
         <v>98</v>
@@ -1471,16 +1495,16 @@
         <v>97</v>
       </c>
       <c r="H4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I4" t="s">
         <v>122</v>
       </c>
       <c r="J4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L4" t="s">
         <v>112</v>
@@ -1515,10 +1539,10 @@
       <c r="X4" s="1">
         <v>4</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4">
         <v>4</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4">
         <v>6</v>
       </c>
       <c r="AA4">
@@ -1551,35 +1575,38 @@
       <c r="AM4" s="1">
         <v>6</v>
       </c>
+      <c r="AQ4" t="s">
+        <v>140</v>
+      </c>
       <c r="AS4" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AT4" t="s">
         <v>108</v>
       </c>
       <c r="AV4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AW4" t="s">
         <v>110</v>
       </c>
       <c r="AX4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AY4" t="s">
         <v>118</v>
       </c>
       <c r="AZ4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="BA4" t="s">
         <v>112</v>
       </c>
       <c r="BC4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="BD4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BE4" t="s">
         <v>108</v>
@@ -1588,10 +1615,10 @@
         <v>95</v>
       </c>
       <c r="CA4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="CV4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:100" x14ac:dyDescent="0.25">
@@ -1605,10 +1632,10 @@
         <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F5" t="s">
         <v>98</v>
@@ -1623,10 +1650,10 @@
         <v>98</v>
       </c>
       <c r="J5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="L5" t="s">
         <v>95</v>
@@ -1635,7 +1662,7 @@
         <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="P5" s="1">
         <v>2</v>
@@ -1664,10 +1691,10 @@
       <c r="X5" s="1">
         <v>2</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Y5">
         <v>4</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="Z5">
         <v>5</v>
       </c>
       <c r="AA5">
@@ -1700,8 +1727,11 @@
       <c r="AK5" s="1">
         <v>4</v>
       </c>
+      <c r="AQ5" t="s">
+        <v>148</v>
+      </c>
       <c r="AS5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="AW5" t="s">
         <v>110</v>
@@ -1713,40 +1743,40 @@
         <v>95</v>
       </c>
       <c r="BI5" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="BJ5" t="s">
         <v>95</v>
       </c>
       <c r="BR5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="BS5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="BT5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BU5" t="s">
         <v>108</v>
       </c>
       <c r="BV5" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="BW5" t="s">
         <v>118</v>
       </c>
       <c r="BX5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="BY5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="BZ5" t="s">
         <v>112</v>
       </c>
       <c r="CV5" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:100" x14ac:dyDescent="0.25">
@@ -1760,37 +1790,37 @@
         <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F6" t="s">
         <v>97</v>
       </c>
       <c r="G6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H6" t="s">
         <v>98</v>
       </c>
       <c r="I6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J6" t="s">
         <v>98</v>
       </c>
       <c r="K6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="L6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="M6">
         <v>3</v>
       </c>
       <c r="N6" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="P6" s="1">
         <v>8</v>
@@ -1819,10 +1849,10 @@
       <c r="X6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y6">
         <v>7</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z6">
         <v>8</v>
       </c>
       <c r="AA6">
@@ -1855,44 +1885,47 @@
       <c r="AM6" s="1">
         <v>6</v>
       </c>
+      <c r="AQ6" t="s">
+        <v>158</v>
+      </c>
       <c r="AS6" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="AV6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AW6" t="s">
         <v>110</v>
       </c>
       <c r="AX6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="BA6" t="s">
         <v>112</v>
       </c>
       <c r="BB6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="BC6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="BD6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BF6" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="BG6" t="s">
         <v>118</v>
       </c>
       <c r="BH6" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="BZ6" t="s">
         <v>112</v>
       </c>
       <c r="CV6" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:100" x14ac:dyDescent="0.25">
@@ -1906,16 +1939,16 @@
         <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F7" t="s">
         <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I7" t="s">
         <v>122</v>
@@ -1924,7 +1957,7 @@
         <v>97</v>
       </c>
       <c r="K7" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="L7" t="s">
         <v>95</v>
@@ -1959,10 +1992,10 @@
       <c r="X7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Y7">
         <v>6</v>
       </c>
-      <c r="Z7" s="2" t="s">
+      <c r="Z7" t="s">
         <v>103</v>
       </c>
       <c r="AA7">
@@ -1989,8 +2022,11 @@
       <c r="AJ7" s="1">
         <v>3</v>
       </c>
+      <c r="AQ7" t="s">
+        <v>162</v>
+      </c>
       <c r="AS7" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AT7" t="s">
         <v>108</v>
@@ -1999,13 +2035,13 @@
         <v>109</v>
       </c>
       <c r="AV7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AW7" t="s">
         <v>110</v>
       </c>
       <c r="AX7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AY7" t="s">
         <v>118</v>
@@ -2017,26 +2053,25 @@
         <v>95</v>
       </c>
       <c r="BR7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="BS7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="BT7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="BY7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="BZ7" t="s">
         <v>112</v>
       </c>
       <c r="CV7" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>